<commit_message>
Added get_report_stats() to excel_Parsing which returns the gender and department stats of excel sheet
</commit_message>
<xml_diff>
--- a/Case tracking for CS class.xlsx
+++ b/Case tracking for CS class.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dianezg\Box\Diane@CGE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nitef\OneDrive\Desktop\visas\222\Visa-Dashboard-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EAAE4E-8393-4A34-A0BB-12214ED3405F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E881B9BA-5E5A-4543-B4C3-FF6EEA65E1AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Current H-1B cases" sheetId="9" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="436">
   <si>
     <t>First Name</t>
   </si>
@@ -1519,6 +1519,30 @@
   </si>
   <si>
     <t>Department Advisor/PI/chair</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>female</t>
   </si>
 </sst>
 </file>
@@ -2760,40 +2784,40 @@
   </sheetPr>
   <dimension ref="A1:CD120"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X2" sqref="X2"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U27" sqref="U27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" style="157" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" style="157" customWidth="1"/>
-    <col min="3" max="4" width="28.85546875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" style="157" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" style="157" customWidth="1"/>
+    <col min="3" max="4" width="28.88671875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="11" customWidth="1"/>
     <col min="7" max="8" width="14" style="11" customWidth="1"/>
     <col min="9" max="9" width="52" style="157" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="83" style="166" customWidth="1"/>
-    <col min="11" max="11" width="43.85546875" style="167" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" style="168" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" style="169" customWidth="1"/>
-    <col min="14" max="14" width="25.42578125" style="169" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" style="170" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.42578125" style="168" customWidth="1"/>
-    <col min="17" max="17" width="15.85546875" style="11" customWidth="1"/>
-    <col min="18" max="18" width="68.7109375" style="157" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" style="165" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.7109375" style="165" customWidth="1"/>
-    <col min="21" max="21" width="28.140625" style="165" customWidth="1"/>
-    <col min="22" max="23" width="20.140625" style="165" customWidth="1"/>
+    <col min="11" max="11" width="43.88671875" style="167" customWidth="1"/>
+    <col min="12" max="12" width="18.109375" style="168" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" style="169" customWidth="1"/>
+    <col min="14" max="14" width="25.44140625" style="169" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" style="170" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.44140625" style="168" customWidth="1"/>
+    <col min="17" max="17" width="15.88671875" style="11" customWidth="1"/>
+    <col min="18" max="18" width="68.6640625" style="157" customWidth="1"/>
+    <col min="19" max="19" width="16.6640625" style="165" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.6640625" style="165" customWidth="1"/>
+    <col min="21" max="21" width="28.109375" style="165" customWidth="1"/>
+    <col min="22" max="23" width="20.109375" style="165" customWidth="1"/>
     <col min="24" max="24" width="22" style="165" customWidth="1"/>
-    <col min="25" max="26" width="13.42578125" style="155" customWidth="1"/>
+    <col min="25" max="26" width="13.44140625" style="155" customWidth="1"/>
     <col min="27" max="27" width="37" style="165" customWidth="1"/>
-    <col min="28" max="16384" width="9.140625" style="11"/>
+    <col min="28" max="16384" width="9.109375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:82" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>339</v>
       </c>
@@ -2876,7 +2900,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="2" spans="1:82" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:82" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>364</v>
       </c>
@@ -2892,7 +2916,9 @@
         <v>33</v>
       </c>
       <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="H2" s="21" t="s">
+        <v>428</v>
+      </c>
       <c r="I2" s="21" t="s">
         <v>171</v>
       </c>
@@ -2993,7 +3019,7 @@
       <c r="CC2" s="33"/>
       <c r="CD2" s="33"/>
     </row>
-    <row r="3" spans="1:82" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:82" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>364</v>
       </c>
@@ -3005,7 +3031,9 @@
       <c r="E3" s="21"/>
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
+      <c r="H3" s="21" t="s">
+        <v>429</v>
+      </c>
       <c r="I3" s="21" t="s">
         <v>18</v>
       </c>
@@ -3085,7 +3113,7 @@
       <c r="CC3" s="33"/>
       <c r="CD3" s="33"/>
     </row>
-    <row r="4" spans="1:82" s="33" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:82" s="33" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>340</v>
       </c>
@@ -3101,7 +3129,9 @@
         <v>24</v>
       </c>
       <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
+      <c r="H4" s="12" t="s">
+        <v>430</v>
+      </c>
       <c r="I4" s="35" t="s">
         <v>171</v>
       </c>
@@ -3145,7 +3175,7 @@
         <v>Philosophy</v>
       </c>
     </row>
-    <row r="5" spans="1:82" s="33" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:82" s="33" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
         <v>340</v>
       </c>
@@ -3161,7 +3191,9 @@
         <v>24</v>
       </c>
       <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
+      <c r="H5" s="36" t="s">
+        <v>431</v>
+      </c>
       <c r="I5" s="36" t="s">
         <v>8</v>
       </c>
@@ -3202,7 +3234,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="6" spans="1:82" s="33" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:82" s="33" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
         <v>340</v>
       </c>
@@ -3218,7 +3250,9 @@
         <v>24</v>
       </c>
       <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="H6" s="12" t="s">
+        <v>431</v>
+      </c>
       <c r="I6" s="35" t="s">
         <v>8</v>
       </c>
@@ -3267,7 +3301,7 @@
         <v>Philosophy</v>
       </c>
     </row>
-    <row r="7" spans="1:82" s="33" customFormat="1" ht="345" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:82" s="33" customFormat="1" ht="345" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
         <v>340</v>
       </c>
@@ -3283,7 +3317,9 @@
         <v>24</v>
       </c>
       <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
+      <c r="H7" s="12" t="s">
+        <v>431</v>
+      </c>
       <c r="I7" s="35" t="s">
         <v>186</v>
       </c>
@@ -3315,7 +3351,7 @@
         <v>Philosophy</v>
       </c>
     </row>
-    <row r="8" spans="1:82" s="56" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:82" s="56" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>341</v>
       </c>
@@ -3331,7 +3367,9 @@
         <v>5</v>
       </c>
       <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="H8" s="21" t="s">
+        <v>432</v>
+      </c>
       <c r="I8" s="21" t="s">
         <v>40</v>
       </c>
@@ -3437,7 +3475,7 @@
       <c r="CC8" s="11"/>
       <c r="CD8" s="11"/>
     </row>
-    <row r="9" spans="1:82" s="34" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:82" s="34" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>341</v>
       </c>
@@ -3453,7 +3491,9 @@
         <v>5</v>
       </c>
       <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+      <c r="H9" s="21" t="s">
+        <v>433</v>
+      </c>
       <c r="I9" s="19" t="s">
         <v>18</v>
       </c>
@@ -3533,7 +3573,7 @@
       <c r="CC9" s="33"/>
       <c r="CD9" s="33"/>
     </row>
-    <row r="10" spans="1:82" s="33" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:82" s="33" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
         <v>342</v>
       </c>
@@ -3549,7 +3589,9 @@
         <v>382</v>
       </c>
       <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
+      <c r="H10" s="12" t="s">
+        <v>434</v>
+      </c>
       <c r="I10" s="35" t="s">
         <v>171</v>
       </c>
@@ -3591,7 +3633,7 @@
         <v>Dance</v>
       </c>
     </row>
-    <row r="11" spans="1:82" s="33" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:82" s="33" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
         <v>342</v>
       </c>
@@ -3607,7 +3649,9 @@
         <v>382</v>
       </c>
       <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
+      <c r="H11" s="12" t="s">
+        <v>434</v>
+      </c>
       <c r="I11" s="35" t="s">
         <v>17</v>
       </c>
@@ -3651,7 +3695,7 @@
         <v>Dance</v>
       </c>
     </row>
-    <row r="12" spans="1:82" s="33" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:82" s="33" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="35" t="s">
         <v>342</v>
       </c>
@@ -3667,7 +3711,9 @@
         <v>382</v>
       </c>
       <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
+      <c r="H12" s="12" t="s">
+        <v>434</v>
+      </c>
       <c r="I12" s="35" t="s">
         <v>383</v>
       </c>
@@ -3711,7 +3757,7 @@
         <v>Dance</v>
       </c>
     </row>
-    <row r="13" spans="1:82" s="33" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:82" s="33" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
         <v>342</v>
       </c>
@@ -3727,7 +3773,9 @@
         <v>382</v>
       </c>
       <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
+      <c r="H13" s="12" t="s">
+        <v>435</v>
+      </c>
       <c r="I13" s="35" t="s">
         <v>380</v>
       </c>
@@ -3774,7 +3822,7 @@
         <v>Dance</v>
       </c>
     </row>
-    <row r="14" spans="1:82" s="33" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:82" s="33" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
         <v>342</v>
       </c>
@@ -3790,7 +3838,9 @@
         <v>382</v>
       </c>
       <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
+      <c r="H14" s="12" t="s">
+        <v>435</v>
+      </c>
       <c r="I14" s="35" t="s">
         <v>18</v>
       </c>
@@ -3817,7 +3867,7 @@
       <c r="Z14" s="45"/>
       <c r="AA14" s="62"/>
     </row>
-    <row r="15" spans="1:82" s="34" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:82" s="34" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="57" t="s">
         <v>300</v>
       </c>
@@ -3833,7 +3883,9 @@
         <v>37</v>
       </c>
       <c r="G15" s="63"/>
-      <c r="H15" s="63"/>
+      <c r="H15" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I15" s="57" t="s">
         <v>181</v>
       </c>
@@ -3934,7 +3986,7 @@
       <c r="CC15" s="33"/>
       <c r="CD15" s="33"/>
     </row>
-    <row r="16" spans="1:82" s="72" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:82" s="72" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="57" t="s">
         <v>300</v>
       </c>
@@ -3946,7 +3998,9 @@
       <c r="E16" s="69"/>
       <c r="F16" s="69"/>
       <c r="G16" s="69"/>
-      <c r="H16" s="69"/>
+      <c r="H16" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I16" s="57" t="s">
         <v>18</v>
       </c>
@@ -4026,7 +4080,7 @@
       <c r="CC16" s="71"/>
       <c r="CD16" s="71"/>
     </row>
-    <row r="17" spans="1:82" s="33" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:82" s="33" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="35" t="s">
         <v>301</v>
       </c>
@@ -4040,7 +4094,9 @@
       </c>
       <c r="F17" s="35"/>
       <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
+      <c r="H17" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I17" s="36" t="s">
         <v>40</v>
       </c>
@@ -4075,7 +4131,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:82" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:82" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="35" t="s">
         <v>301</v>
       </c>
@@ -4089,7 +4145,9 @@
       </c>
       <c r="F18" s="35"/>
       <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
+      <c r="H18" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I18" s="73" t="s">
         <v>122</v>
       </c>
@@ -4119,7 +4177,7 @@
       <c r="Z18" s="45"/>
       <c r="AA18" s="62"/>
     </row>
-    <row r="19" spans="1:82" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:82" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="35" t="s">
         <v>301</v>
       </c>
@@ -4133,7 +4191,9 @@
       </c>
       <c r="F19" s="35"/>
       <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
+      <c r="H19" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I19" s="35" t="s">
         <v>18</v>
       </c>
@@ -4158,7 +4218,7 @@
       <c r="Z19" s="45"/>
       <c r="AA19" s="62"/>
     </row>
-    <row r="20" spans="1:82" s="34" customFormat="1" ht="255" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:82" s="34" customFormat="1" ht="255" x14ac:dyDescent="0.25">
       <c r="A20" s="57" t="s">
         <v>191</v>
       </c>
@@ -4172,7 +4232,9 @@
       </c>
       <c r="F20" s="57"/>
       <c r="G20" s="63"/>
-      <c r="H20" s="63"/>
+      <c r="H20" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I20" s="57" t="s">
         <v>178</v>
       </c>
@@ -4252,7 +4314,7 @@
       <c r="CC20" s="33"/>
       <c r="CD20" s="33"/>
     </row>
-    <row r="21" spans="1:82" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:82" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="77" t="s">
         <v>217</v>
       </c>
@@ -4268,7 +4330,9 @@
         <v>33</v>
       </c>
       <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
+      <c r="H21" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I21" s="77" t="s">
         <v>51</v>
       </c>
@@ -4306,7 +4370,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:82" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:82" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="77" t="s">
         <v>217</v>
       </c>
@@ -4322,7 +4386,9 @@
         <v>33</v>
       </c>
       <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
+      <c r="H22" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I22" s="77" t="s">
         <v>179</v>
       </c>
@@ -4347,7 +4413,7 @@
       <c r="Z22" s="45"/>
       <c r="AA22" s="81"/>
     </row>
-    <row r="23" spans="1:82" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:82" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="77" t="s">
         <v>217</v>
       </c>
@@ -4361,7 +4427,9 @@
       </c>
       <c r="F23" s="37"/>
       <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
+      <c r="H23" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I23" s="77" t="s">
         <v>18</v>
       </c>
@@ -4388,7 +4456,7 @@
       <c r="Z23" s="45"/>
       <c r="AA23" s="81"/>
     </row>
-    <row r="24" spans="1:82" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:82" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="57" t="s">
         <v>35</v>
       </c>
@@ -4404,7 +4472,9 @@
         <v>5</v>
       </c>
       <c r="G24" s="63"/>
-      <c r="H24" s="63"/>
+      <c r="H24" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I24" s="57" t="s">
         <v>165</v>
       </c>
@@ -4492,7 +4562,7 @@
       <c r="CC24" s="33"/>
       <c r="CD24" s="33"/>
     </row>
-    <row r="25" spans="1:82" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:82" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="57" t="s">
         <v>35</v>
       </c>
@@ -4508,7 +4578,9 @@
         <v>5</v>
       </c>
       <c r="G25" s="63"/>
-      <c r="H25" s="63"/>
+      <c r="H25" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I25" s="57" t="s">
         <v>8</v>
       </c>
@@ -4601,7 +4673,7 @@
       <c r="CC25" s="33"/>
       <c r="CD25" s="33"/>
     </row>
-    <row r="26" spans="1:82" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:82" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="57" t="s">
         <v>35</v>
       </c>
@@ -4613,7 +4685,9 @@
       <c r="E26" s="64"/>
       <c r="F26" s="57"/>
       <c r="G26" s="63"/>
-      <c r="H26" s="63"/>
+      <c r="H26" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I26" s="57" t="s">
         <v>18</v>
       </c>
@@ -4691,7 +4765,7 @@
       <c r="CC26" s="33"/>
       <c r="CD26" s="33"/>
     </row>
-    <row r="27" spans="1:82" s="33" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:82" s="33" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="35" t="s">
         <v>218</v>
       </c>
@@ -4707,7 +4781,9 @@
         <v>161</v>
       </c>
       <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
+      <c r="H27" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I27" s="35" t="s">
         <v>181</v>
       </c>
@@ -4755,7 +4831,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="28" spans="1:82" s="33" customFormat="1" ht="120" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:82" s="33" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" s="35" t="s">
         <v>218</v>
       </c>
@@ -4769,7 +4845,9 @@
       </c>
       <c r="F28" s="35"/>
       <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
+      <c r="H28" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I28" s="35" t="s">
         <v>18</v>
       </c>
@@ -4794,7 +4872,7 @@
       <c r="Z28" s="45"/>
       <c r="AA28" s="61"/>
     </row>
-    <row r="29" spans="1:82" s="34" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:82" s="34" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="75" t="s">
         <v>354</v>
       </c>
@@ -4810,7 +4888,9 @@
         <v>5</v>
       </c>
       <c r="G29" s="63"/>
-      <c r="H29" s="63"/>
+      <c r="H29" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I29" s="75" t="s">
         <v>40</v>
       </c>
@@ -4907,7 +4987,7 @@
       <c r="CC29" s="33"/>
       <c r="CD29" s="33"/>
     </row>
-    <row r="30" spans="1:82" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:82" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="75" t="s">
         <v>354</v>
       </c>
@@ -4921,7 +5001,9 @@
       </c>
       <c r="F30" s="63"/>
       <c r="G30" s="63"/>
-      <c r="H30" s="63"/>
+      <c r="H30" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I30" s="75" t="s">
         <v>18</v>
       </c>
@@ -5003,7 +5085,7 @@
       <c r="CC30" s="33"/>
       <c r="CD30" s="33"/>
     </row>
-    <row r="31" spans="1:82" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:82" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="86" t="s">
         <v>271</v>
       </c>
@@ -5019,7 +5101,9 @@
         <v>24</v>
       </c>
       <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
+      <c r="H31" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I31" s="86" t="s">
         <v>384</v>
       </c>
@@ -5055,7 +5139,7 @@
       <c r="Z31" s="45"/>
       <c r="AA31" s="62"/>
     </row>
-    <row r="32" spans="1:82" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:82" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="86" t="s">
         <v>271</v>
       </c>
@@ -5067,7 +5151,9 @@
       <c r="E32" s="37"/>
       <c r="F32" s="12"/>
       <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
+      <c r="H32" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I32" s="86" t="s">
         <v>18</v>
       </c>
@@ -5092,7 +5178,7 @@
       <c r="Z32" s="45"/>
       <c r="AA32" s="62"/>
     </row>
-    <row r="33" spans="1:82" s="99" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:82" s="99" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="89" t="s">
         <v>192</v>
       </c>
@@ -5108,7 +5194,9 @@
         <v>41</v>
       </c>
       <c r="G33" s="90"/>
-      <c r="H33" s="90"/>
+      <c r="H33" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I33" s="89" t="s">
         <v>171</v>
       </c>
@@ -5196,7 +5284,7 @@
       <c r="CC33" s="33"/>
       <c r="CD33" s="33"/>
     </row>
-    <row r="34" spans="1:82" s="99" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:82" s="99" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="89" t="s">
         <v>192</v>
       </c>
@@ -5212,7 +5300,9 @@
         <v>41</v>
       </c>
       <c r="G34" s="90"/>
-      <c r="H34" s="90"/>
+      <c r="H34" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I34" s="89" t="s">
         <v>8</v>
       </c>
@@ -5303,7 +5393,7 @@
       <c r="CC34" s="33"/>
       <c r="CD34" s="33"/>
     </row>
-    <row r="35" spans="1:82" s="99" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:82" s="99" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="89" t="s">
         <v>192</v>
       </c>
@@ -5315,7 +5405,9 @@
       <c r="E35" s="91"/>
       <c r="F35" s="90"/>
       <c r="G35" s="90"/>
-      <c r="H35" s="90"/>
+      <c r="H35" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I35" s="89" t="s">
         <v>18</v>
       </c>
@@ -5395,7 +5487,7 @@
       <c r="CC35" s="33"/>
       <c r="CD35" s="33"/>
     </row>
-    <row r="36" spans="1:82" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:82" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="57" t="s">
         <v>43</v>
       </c>
@@ -5411,7 +5503,9 @@
         <v>23</v>
       </c>
       <c r="G36" s="63"/>
-      <c r="H36" s="63"/>
+      <c r="H36" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I36" s="57" t="s">
         <v>366</v>
       </c>
@@ -5507,7 +5601,7 @@
       <c r="CC36" s="33"/>
       <c r="CD36" s="33"/>
     </row>
-    <row r="37" spans="1:82" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:82" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="57" t="s">
         <v>43</v>
       </c>
@@ -5523,7 +5617,9 @@
         <v>23</v>
       </c>
       <c r="G37" s="63"/>
-      <c r="H37" s="63"/>
+      <c r="H37" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I37" s="57" t="s">
         <v>8</v>
       </c>
@@ -5619,7 +5715,7 @@
       <c r="CC37" s="33"/>
       <c r="CD37" s="33"/>
     </row>
-    <row r="38" spans="1:82" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:82" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="57" t="s">
         <v>43</v>
       </c>
@@ -5635,7 +5731,9 @@
         <v>23</v>
       </c>
       <c r="G38" s="63"/>
-      <c r="H38" s="63"/>
+      <c r="H38" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I38" s="57" t="s">
         <v>130</v>
       </c>
@@ -5734,7 +5832,7 @@
       <c r="CC38" s="33"/>
       <c r="CD38" s="33"/>
     </row>
-    <row r="39" spans="1:82" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:82" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="57" t="s">
         <v>43</v>
       </c>
@@ -5750,7 +5848,9 @@
         <v>23</v>
       </c>
       <c r="G39" s="63"/>
-      <c r="H39" s="63"/>
+      <c r="H39" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I39" s="57" t="s">
         <v>18</v>
       </c>
@@ -5830,7 +5930,7 @@
       <c r="CC39" s="33"/>
       <c r="CD39" s="33"/>
     </row>
-    <row r="40" spans="1:82" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:82" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="35" t="s">
         <v>353</v>
       </c>
@@ -5846,7 +5946,9 @@
         <v>32</v>
       </c>
       <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
+      <c r="H40" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I40" s="35" t="s">
         <v>40</v>
       </c>
@@ -5882,7 +5984,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="41" spans="1:82" s="33" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:82" s="33" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="35" t="s">
         <v>353</v>
       </c>
@@ -5894,7 +5996,9 @@
       <c r="E41" s="37"/>
       <c r="F41" s="35"/>
       <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
+      <c r="H41" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I41" s="35" t="s">
         <v>18</v>
       </c>
@@ -5921,7 +6025,7 @@
       <c r="Z41" s="45"/>
       <c r="AA41" s="62"/>
     </row>
-    <row r="42" spans="1:82" s="56" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:82" s="56" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="57" t="s">
         <v>349</v>
       </c>
@@ -5937,7 +6041,9 @@
         <v>47</v>
       </c>
       <c r="G42" s="63"/>
-      <c r="H42" s="63"/>
+      <c r="H42" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I42" s="57" t="s">
         <v>171</v>
       </c>
@@ -6033,7 +6139,7 @@
       <c r="CC42" s="11"/>
       <c r="CD42" s="11"/>
     </row>
-    <row r="43" spans="1:82" s="56" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:82" s="56" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="57" t="s">
         <v>349</v>
       </c>
@@ -6049,7 +6155,9 @@
         <v>47</v>
       </c>
       <c r="G43" s="21"/>
-      <c r="H43" s="21"/>
+      <c r="H43" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I43" s="21" t="s">
         <v>8</v>
       </c>
@@ -6147,7 +6255,7 @@
       <c r="CC43" s="11"/>
       <c r="CD43" s="11"/>
     </row>
-    <row r="44" spans="1:82" s="56" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:82" s="56" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="57" t="s">
         <v>349</v>
       </c>
@@ -6163,7 +6271,9 @@
         <v>47</v>
       </c>
       <c r="G44" s="21"/>
-      <c r="H44" s="21"/>
+      <c r="H44" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I44" s="21" t="s">
         <v>381</v>
       </c>
@@ -6262,7 +6372,7 @@
       <c r="CC44" s="11"/>
       <c r="CD44" s="11"/>
     </row>
-    <row r="45" spans="1:82" s="34" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:82" s="34" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="57" t="s">
         <v>349</v>
       </c>
@@ -6278,7 +6388,9 @@
         <v>47</v>
       </c>
       <c r="G45" s="21"/>
-      <c r="H45" s="21"/>
+      <c r="H45" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I45" s="21" t="s">
         <v>18</v>
       </c>
@@ -6362,7 +6474,7 @@
       <c r="CC45" s="33"/>
       <c r="CD45" s="33"/>
     </row>
-    <row r="46" spans="1:82" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:82" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="35" t="s">
         <v>351</v>
       </c>
@@ -6378,7 +6490,9 @@
         <v>27</v>
       </c>
       <c r="G46" s="36"/>
-      <c r="H46" s="36"/>
+      <c r="H46" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I46" s="35" t="s">
         <v>366</v>
       </c>
@@ -6410,7 +6524,7 @@
       <c r="Z46" s="45"/>
       <c r="AA46" s="46"/>
     </row>
-    <row r="47" spans="1:82" s="33" customFormat="1" ht="135" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:82" s="33" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A47" s="35" t="s">
         <v>351</v>
       </c>
@@ -6426,7 +6540,9 @@
         <v>27</v>
       </c>
       <c r="G47" s="36"/>
-      <c r="H47" s="36"/>
+      <c r="H47" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I47" s="35" t="s">
         <v>18</v>
       </c>
@@ -6451,7 +6567,7 @@
       <c r="Z47" s="45"/>
       <c r="AA47" s="46"/>
     </row>
-    <row r="48" spans="1:82" s="34" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:82" s="34" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="57" t="s">
         <v>344</v>
       </c>
@@ -6463,7 +6579,9 @@
       <c r="E48" s="64"/>
       <c r="F48" s="57"/>
       <c r="G48" s="21"/>
-      <c r="H48" s="21"/>
+      <c r="H48" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I48" s="57" t="s">
         <v>366</v>
       </c>
@@ -6566,7 +6684,7 @@
       <c r="CC48" s="33"/>
       <c r="CD48" s="33"/>
     </row>
-    <row r="49" spans="1:82" s="34" customFormat="1" ht="210" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:82" s="34" customFormat="1" ht="210" x14ac:dyDescent="0.25">
       <c r="A49" s="57" t="s">
         <v>344</v>
       </c>
@@ -6580,7 +6698,9 @@
       </c>
       <c r="F49" s="57"/>
       <c r="G49" s="21"/>
-      <c r="H49" s="21"/>
+      <c r="H49" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I49" s="57" t="s">
         <v>18</v>
       </c>
@@ -6660,7 +6780,7 @@
       <c r="CC49" s="33"/>
       <c r="CD49" s="33"/>
     </row>
-    <row r="50" spans="1:82" s="108" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:82" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="35" t="s">
         <v>344</v>
       </c>
@@ -6676,7 +6796,9 @@
         <v>23</v>
       </c>
       <c r="G50" s="12"/>
-      <c r="H50" s="12"/>
+      <c r="H50" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I50" s="35" t="s">
         <v>366</v>
       </c>
@@ -6712,7 +6834,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:82" s="108" customFormat="1" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:82" s="108" customFormat="1" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A51" s="35" t="s">
         <v>344</v>
       </c>
@@ -6728,7 +6850,9 @@
         <v>23</v>
       </c>
       <c r="G51" s="12"/>
-      <c r="H51" s="12"/>
+      <c r="H51" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I51" s="35" t="s">
         <v>18</v>
       </c>
@@ -6757,7 +6881,7 @@
       <c r="Z51" s="45"/>
       <c r="AA51" s="62"/>
     </row>
-    <row r="52" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="57" t="s">
         <v>389</v>
       </c>
@@ -6775,7 +6899,9 @@
       <c r="G52" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="H52" s="63"/>
+      <c r="H52" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I52" s="57" t="s">
         <v>171</v>
       </c>
@@ -6870,7 +6996,7 @@
       <c r="CC52" s="11"/>
       <c r="CD52" s="11"/>
     </row>
-    <row r="53" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="57" t="s">
         <v>389</v>
       </c>
@@ -6884,7 +7010,9 @@
       </c>
       <c r="F53" s="57"/>
       <c r="G53" s="63"/>
-      <c r="H53" s="63"/>
+      <c r="H53" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I53" s="57" t="s">
         <v>365</v>
       </c>
@@ -6966,7 +7094,7 @@
       <c r="CC53" s="11"/>
       <c r="CD53" s="11"/>
     </row>
-    <row r="54" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="57" t="s">
         <v>389</v>
       </c>
@@ -6980,7 +7108,9 @@
       </c>
       <c r="F54" s="57"/>
       <c r="G54" s="63"/>
-      <c r="H54" s="63"/>
+      <c r="H54" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I54" s="57" t="s">
         <v>18</v>
       </c>
@@ -7060,7 +7190,7 @@
       <c r="CC54" s="11"/>
       <c r="CD54" s="11"/>
     </row>
-    <row r="55" spans="1:82" ht="45" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:82" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="53" t="s">
         <v>390</v>
       </c>
@@ -7078,7 +7208,9 @@
       <c r="G55" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="H55" s="36"/>
+      <c r="H55" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I55" s="53" t="s">
         <v>368</v>
       </c>
@@ -7121,7 +7253,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:82" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A56" s="53" t="s">
         <v>390</v>
       </c>
@@ -7139,7 +7271,9 @@
       <c r="G56" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="H56" s="36"/>
+      <c r="H56" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I56" s="53" t="s">
         <v>8</v>
       </c>
@@ -7169,7 +7303,7 @@
       <c r="Z56" s="45"/>
       <c r="AA56" s="46"/>
     </row>
-    <row r="57" spans="1:82" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A57" s="53" t="s">
         <v>390</v>
       </c>
@@ -7187,7 +7321,9 @@
       <c r="G57" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="H57" s="36"/>
+      <c r="H57" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I57" s="53" t="s">
         <v>18</v>
       </c>
@@ -7216,7 +7352,7 @@
       </c>
       <c r="AA57" s="46"/>
     </row>
-    <row r="58" spans="1:82" s="56" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:82" s="56" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
         <v>337</v>
       </c>
@@ -7234,7 +7370,9 @@
       <c r="G58" s="21" t="s">
         <v>369</v>
       </c>
-      <c r="H58" s="21"/>
+      <c r="H58" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I58" s="21" t="s">
         <v>379</v>
       </c>
@@ -7334,7 +7472,7 @@
       <c r="CC58" s="11"/>
       <c r="CD58" s="11"/>
     </row>
-    <row r="59" spans="1:82" s="56" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:82" s="56" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="19" t="s">
         <v>337</v>
       </c>
@@ -7350,7 +7488,9 @@
         <v>229</v>
       </c>
       <c r="G59" s="21"/>
-      <c r="H59" s="21"/>
+      <c r="H59" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I59" s="19" t="s">
         <v>8</v>
       </c>
@@ -7451,7 +7591,7 @@
       <c r="CC59" s="11"/>
       <c r="CD59" s="11"/>
     </row>
-    <row r="60" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="19" t="s">
         <v>337</v>
       </c>
@@ -7463,7 +7603,9 @@
       <c r="E60" s="21"/>
       <c r="F60" s="21"/>
       <c r="G60" s="21"/>
-      <c r="H60" s="21"/>
+      <c r="H60" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I60" s="75" t="s">
         <v>18</v>
       </c>
@@ -7541,7 +7683,7 @@
       <c r="CC60" s="11"/>
       <c r="CD60" s="11"/>
     </row>
-    <row r="61" spans="1:82" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A61" s="86" t="s">
         <v>336</v>
       </c>
@@ -7557,7 +7699,9 @@
         <v>5</v>
       </c>
       <c r="G61" s="12"/>
-      <c r="H61" s="12"/>
+      <c r="H61" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I61" s="86" t="s">
         <v>51</v>
       </c>
@@ -7591,7 +7735,7 @@
       <c r="Z61" s="45"/>
       <c r="AA61" s="81"/>
     </row>
-    <row r="62" spans="1:82" ht="30" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:82" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="86" t="s">
         <v>336</v>
       </c>
@@ -7603,7 +7747,9 @@
       <c r="E62" s="37"/>
       <c r="F62" s="12"/>
       <c r="G62" s="12"/>
-      <c r="H62" s="12"/>
+      <c r="H62" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I62" s="86" t="s">
         <v>18</v>
       </c>
@@ -7628,7 +7774,7 @@
       <c r="Z62" s="45"/>
       <c r="AA62" s="81"/>
     </row>
-    <row r="63" spans="1:82" s="56" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:82" s="56" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="75" t="s">
         <v>334</v>
       </c>
@@ -7644,7 +7790,9 @@
         <v>7</v>
       </c>
       <c r="G63" s="63"/>
-      <c r="H63" s="63"/>
+      <c r="H63" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I63" s="75" t="s">
         <v>165</v>
       </c>
@@ -7747,7 +7895,7 @@
       <c r="CC63" s="11"/>
       <c r="CD63" s="11"/>
     </row>
-    <row r="64" spans="1:82" s="56" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:82" s="56" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A64" s="75" t="s">
         <v>334</v>
       </c>
@@ -7761,7 +7909,9 @@
       </c>
       <c r="F64" s="63"/>
       <c r="G64" s="63"/>
-      <c r="H64" s="63"/>
+      <c r="H64" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I64" s="75" t="s">
         <v>18</v>
       </c>
@@ -7841,7 +7991,7 @@
       <c r="CC64" s="11"/>
       <c r="CD64" s="11"/>
     </row>
-    <row r="65" spans="1:82" ht="45" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:82" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="86" t="s">
         <v>203</v>
       </c>
@@ -7857,7 +8007,9 @@
         <v>5</v>
       </c>
       <c r="G65" s="12"/>
-      <c r="H65" s="12"/>
+      <c r="H65" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I65" s="86" t="s">
         <v>51</v>
       </c>
@@ -7897,7 +8049,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="66" spans="1:82" ht="285" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:82" ht="285" x14ac:dyDescent="0.25">
       <c r="A66" s="86" t="s">
         <v>203</v>
       </c>
@@ -7911,7 +8063,9 @@
       </c>
       <c r="F66" s="12"/>
       <c r="G66" s="12"/>
-      <c r="H66" s="12"/>
+      <c r="H66" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I66" s="86" t="s">
         <v>18</v>
       </c>
@@ -7936,7 +8090,7 @@
       <c r="Z66" s="45"/>
       <c r="AA66" s="81"/>
     </row>
-    <row r="67" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="75" t="s">
         <v>330</v>
       </c>
@@ -7952,7 +8106,9 @@
         <v>5</v>
       </c>
       <c r="G67" s="63"/>
-      <c r="H67" s="63"/>
+      <c r="H67" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I67" s="75" t="s">
         <v>165</v>
       </c>
@@ -8041,7 +8197,7 @@
       <c r="CC67" s="11"/>
       <c r="CD67" s="11"/>
     </row>
-    <row r="68" spans="1:82" s="56" customFormat="1" ht="135" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:82" s="56" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A68" s="75" t="s">
         <v>330</v>
       </c>
@@ -8055,7 +8211,9 @@
       </c>
       <c r="F68" s="63"/>
       <c r="G68" s="63"/>
-      <c r="H68" s="63"/>
+      <c r="H68" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I68" s="75" t="s">
         <v>18</v>
       </c>
@@ -8135,7 +8293,7 @@
       <c r="CC68" s="11"/>
       <c r="CD68" s="11"/>
     </row>
-    <row r="69" spans="1:82" ht="60" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:82" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" s="86" t="s">
         <v>312</v>
       </c>
@@ -8151,7 +8309,9 @@
         <v>284</v>
       </c>
       <c r="G69" s="12"/>
-      <c r="H69" s="12"/>
+      <c r="H69" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I69" s="86" t="s">
         <v>165</v>
       </c>
@@ -8187,7 +8347,7 @@
       </c>
       <c r="AA69" s="81"/>
     </row>
-    <row r="70" spans="1:82" ht="30" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:82" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="86" t="s">
         <v>312</v>
       </c>
@@ -8201,7 +8361,9 @@
       </c>
       <c r="F70" s="12"/>
       <c r="G70" s="12"/>
-      <c r="H70" s="12"/>
+      <c r="H70" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I70" s="53" t="s">
         <v>18</v>
       </c>
@@ -8228,7 +8390,7 @@
       <c r="Z70" s="45"/>
       <c r="AA70" s="81"/>
     </row>
-    <row r="71" spans="1:82" s="56" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:82" s="56" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="75" t="s">
         <v>176</v>
       </c>
@@ -8244,7 +8406,9 @@
         <v>5</v>
       </c>
       <c r="G71" s="63"/>
-      <c r="H71" s="63"/>
+      <c r="H71" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I71" s="19" t="s">
         <v>171</v>
       </c>
@@ -8344,7 +8508,7 @@
       <c r="CC71" s="11"/>
       <c r="CD71" s="11"/>
     </row>
-    <row r="72" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="75" t="s">
         <v>176</v>
       </c>
@@ -8358,7 +8522,9 @@
       </c>
       <c r="F72" s="63"/>
       <c r="G72" s="63"/>
-      <c r="H72" s="63"/>
+      <c r="H72" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I72" s="19" t="s">
         <v>18</v>
       </c>
@@ -8438,7 +8604,7 @@
       <c r="CC72" s="11"/>
       <c r="CD72" s="11"/>
     </row>
-    <row r="73" spans="1:82" ht="30" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:82" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="53" t="s">
         <v>232</v>
       </c>
@@ -8452,7 +8618,9 @@
       </c>
       <c r="F73" s="36"/>
       <c r="G73" s="36"/>
-      <c r="H73" s="36"/>
+      <c r="H73" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I73" s="86" t="s">
         <v>165</v>
       </c>
@@ -8492,7 +8660,7 @@
       </c>
       <c r="AA73" s="46"/>
     </row>
-    <row r="74" spans="1:82" ht="45" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:82" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="53" t="s">
         <v>232</v>
       </c>
@@ -8506,7 +8674,9 @@
       </c>
       <c r="F74" s="36"/>
       <c r="G74" s="36"/>
-      <c r="H74" s="36"/>
+      <c r="H74" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I74" s="53" t="s">
         <v>18</v>
       </c>
@@ -8531,7 +8701,7 @@
       <c r="Z74" s="45"/>
       <c r="AA74" s="46"/>
     </row>
-    <row r="75" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="19" t="s">
         <v>53</v>
       </c>
@@ -8547,7 +8717,9 @@
         <v>23</v>
       </c>
       <c r="G75" s="21"/>
-      <c r="H75" s="21"/>
+      <c r="H75" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I75" s="19" t="s">
         <v>40</v>
       </c>
@@ -8640,7 +8812,7 @@
       <c r="CC75" s="11"/>
       <c r="CD75" s="11"/>
     </row>
-    <row r="76" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="19" t="s">
         <v>53</v>
       </c>
@@ -8652,7 +8824,9 @@
       <c r="E76" s="21"/>
       <c r="F76" s="21"/>
       <c r="G76" s="21"/>
-      <c r="H76" s="21"/>
+      <c r="H76" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I76" s="19" t="s">
         <v>186</v>
       </c>
@@ -8732,7 +8906,7 @@
       <c r="CC76" s="11"/>
       <c r="CD76" s="11"/>
     </row>
-    <row r="77" spans="1:82" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A77" s="119" t="s">
         <v>325</v>
       </c>
@@ -8746,7 +8920,9 @@
       </c>
       <c r="F77" s="12"/>
       <c r="G77" s="12"/>
-      <c r="H77" s="12"/>
+      <c r="H77" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I77" s="120" t="s">
         <v>131</v>
       </c>
@@ -8780,7 +8956,7 @@
       </c>
       <c r="AA77" s="62"/>
     </row>
-    <row r="78" spans="1:82" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A78" s="119" t="s">
         <v>325</v>
       </c>
@@ -8794,7 +8970,9 @@
       </c>
       <c r="F78" s="12"/>
       <c r="G78" s="12"/>
-      <c r="H78" s="12"/>
+      <c r="H78" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I78" s="120" t="s">
         <v>8</v>
       </c>
@@ -8821,7 +8999,7 @@
       <c r="Z78" s="45"/>
       <c r="AA78" s="62"/>
     </row>
-    <row r="79" spans="1:82" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A79" s="119" t="s">
         <v>325</v>
       </c>
@@ -8833,7 +9011,9 @@
       <c r="E79" s="36"/>
       <c r="F79" s="12"/>
       <c r="G79" s="12"/>
-      <c r="H79" s="12"/>
+      <c r="H79" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I79" s="53" t="s">
         <v>186</v>
       </c>
@@ -8858,7 +9038,7 @@
       <c r="Z79" s="45"/>
       <c r="AA79" s="62"/>
     </row>
-    <row r="80" spans="1:82" s="56" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:82" s="56" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="122" t="s">
         <v>326</v>
       </c>
@@ -8874,7 +9054,9 @@
         <v>289</v>
       </c>
       <c r="G80" s="63"/>
-      <c r="H80" s="63"/>
+      <c r="H80" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I80" s="123" t="s">
         <v>131</v>
       </c>
@@ -8972,7 +9154,7 @@
       <c r="CC80" s="11"/>
       <c r="CD80" s="11"/>
     </row>
-    <row r="81" spans="1:82" s="56" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:82" s="56" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="122" t="s">
         <v>326</v>
       </c>
@@ -8984,7 +9166,9 @@
       <c r="E81" s="21"/>
       <c r="F81" s="63"/>
       <c r="G81" s="63"/>
-      <c r="H81" s="63"/>
+      <c r="H81" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I81" s="19" t="s">
         <v>186</v>
       </c>
@@ -9064,7 +9248,7 @@
       <c r="CC81" s="11"/>
       <c r="CD81" s="11"/>
     </row>
-    <row r="82" spans="1:82" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A82" s="53" t="s">
         <v>57</v>
       </c>
@@ -9080,7 +9264,9 @@
         <v>23</v>
       </c>
       <c r="G82" s="12"/>
-      <c r="H82" s="36"/>
+      <c r="H82" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I82" s="36" t="s">
         <v>40</v>
       </c>
@@ -9118,7 +9304,7 @@
       </c>
       <c r="AA82" s="46"/>
     </row>
-    <row r="83" spans="1:82" ht="195" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:82" ht="195" x14ac:dyDescent="0.25">
       <c r="A83" s="53" t="s">
         <v>57</v>
       </c>
@@ -9132,7 +9318,9 @@
       </c>
       <c r="F83" s="36"/>
       <c r="G83" s="36"/>
-      <c r="H83" s="36"/>
+      <c r="H83" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I83" s="53" t="s">
         <v>18</v>
       </c>
@@ -9159,7 +9347,7 @@
       <c r="Z83" s="45"/>
       <c r="AA83" s="46"/>
     </row>
-    <row r="84" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="57" t="s">
         <v>323</v>
       </c>
@@ -9175,7 +9363,9 @@
         <v>41</v>
       </c>
       <c r="G84" s="63"/>
-      <c r="H84" s="63"/>
+      <c r="H84" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I84" s="57" t="s">
         <v>171</v>
       </c>
@@ -9266,7 +9456,7 @@
       <c r="CC84" s="11"/>
       <c r="CD84" s="11"/>
     </row>
-    <row r="85" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="57" t="s">
         <v>323</v>
       </c>
@@ -9278,7 +9468,9 @@
       <c r="E85" s="64"/>
       <c r="F85" s="57"/>
       <c r="G85" s="63"/>
-      <c r="H85" s="63"/>
+      <c r="H85" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I85" s="57" t="s">
         <v>18</v>
       </c>
@@ -9358,7 +9550,7 @@
       <c r="CC85" s="11"/>
       <c r="CD85" s="11"/>
     </row>
-    <row r="86" spans="1:82" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:82" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.3">
       <c r="A86" s="35" t="s">
         <v>195</v>
       </c>
@@ -9374,7 +9566,9 @@
         <v>56</v>
       </c>
       <c r="G86" s="12"/>
-      <c r="H86" s="12"/>
+      <c r="H86" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I86" s="36" t="s">
         <v>40</v>
       </c>
@@ -9425,7 +9619,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="87" spans="1:82" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:82" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="35" t="s">
         <v>195</v>
       </c>
@@ -9441,7 +9635,9 @@
         <v>56</v>
       </c>
       <c r="G87" s="12"/>
-      <c r="H87" s="12"/>
+      <c r="H87" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I87" s="35"/>
       <c r="J87" s="38"/>
       <c r="K87" s="39"/>
@@ -9484,7 +9680,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="88" spans="1:82" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:82" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="35" t="s">
         <v>195</v>
       </c>
@@ -9496,7 +9692,9 @@
       <c r="E88" s="37"/>
       <c r="F88" s="35"/>
       <c r="G88" s="12"/>
-      <c r="H88" s="12"/>
+      <c r="H88" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I88" s="35" t="s">
         <v>18</v>
       </c>
@@ -9544,7 +9742,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="89" spans="1:82" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:82" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="57" t="s">
         <v>321</v>
       </c>
@@ -9560,7 +9758,9 @@
         <v>126</v>
       </c>
       <c r="G89" s="63"/>
-      <c r="H89" s="63"/>
+      <c r="H89" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I89" s="57" t="s">
         <v>131</v>
       </c>
@@ -9659,7 +9859,7 @@
       <c r="CC89" s="33"/>
       <c r="CD89" s="33"/>
     </row>
-    <row r="90" spans="1:82" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:82" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="57" t="s">
         <v>321</v>
       </c>
@@ -9671,7 +9871,9 @@
       <c r="E90" s="64"/>
       <c r="F90" s="57"/>
       <c r="G90" s="63"/>
-      <c r="H90" s="63"/>
+      <c r="H90" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I90" s="57" t="s">
         <v>18</v>
       </c>
@@ -9751,7 +9953,7 @@
       <c r="CC90" s="33"/>
       <c r="CD90" s="33"/>
     </row>
-    <row r="91" spans="1:82" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:82" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="35" t="s">
         <v>319</v>
       </c>
@@ -9767,7 +9969,9 @@
         <v>128</v>
       </c>
       <c r="G91" s="12"/>
-      <c r="H91" s="12"/>
+      <c r="H91" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I91" s="35" t="s">
         <v>171</v>
       </c>
@@ -9799,7 +10003,7 @@
       <c r="Z91" s="45"/>
       <c r="AA91" s="62"/>
     </row>
-    <row r="92" spans="1:82" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:82" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="35" t="s">
         <v>319</v>
       </c>
@@ -9811,7 +10015,9 @@
       <c r="E92" s="37"/>
       <c r="F92" s="37"/>
       <c r="G92" s="12"/>
-      <c r="H92" s="12"/>
+      <c r="H92" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I92" s="35" t="s">
         <v>18</v>
       </c>
@@ -9836,7 +10042,7 @@
       <c r="Z92" s="45"/>
       <c r="AA92" s="62"/>
     </row>
-    <row r="93" spans="1:82" s="56" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:82" s="56" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A93" s="19" t="s">
         <v>317</v>
       </c>
@@ -9854,7 +10060,9 @@
       <c r="G93" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H93" s="21"/>
+      <c r="H93" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I93" s="19" t="s">
         <v>367</v>
       </c>
@@ -9954,7 +10162,7 @@
       <c r="CC93" s="11"/>
       <c r="CD93" s="11"/>
     </row>
-    <row r="94" spans="1:82" s="56" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:82" s="56" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A94" s="19" t="s">
         <v>317</v>
       </c>
@@ -9970,7 +10178,9 @@
         <v>5</v>
       </c>
       <c r="G94" s="21"/>
-      <c r="H94" s="21"/>
+      <c r="H94" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I94" s="19" t="s">
         <v>8</v>
       </c>
@@ -10071,7 +10281,7 @@
       <c r="CC94" s="11"/>
       <c r="CD94" s="11"/>
     </row>
-    <row r="95" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="19" t="s">
         <v>317</v>
       </c>
@@ -10083,7 +10293,9 @@
       <c r="E95" s="21"/>
       <c r="F95" s="21"/>
       <c r="G95" s="21"/>
-      <c r="H95" s="21"/>
+      <c r="H95" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I95" s="19" t="s">
         <v>18</v>
       </c>
@@ -10163,7 +10375,7 @@
       <c r="CC95" s="11"/>
       <c r="CD95" s="11"/>
     </row>
-    <row r="96" spans="1:82" ht="45" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:82" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="53" t="s">
         <v>313</v>
       </c>
@@ -10177,7 +10389,9 @@
       </c>
       <c r="F96" s="36"/>
       <c r="G96" s="36"/>
-      <c r="H96" s="36"/>
+      <c r="H96" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I96" s="35" t="s">
         <v>366</v>
       </c>
@@ -10211,7 +10425,7 @@
       <c r="Z96" s="45"/>
       <c r="AA96" s="46"/>
     </row>
-    <row r="97" spans="1:82" ht="315" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:82" ht="315" x14ac:dyDescent="0.25">
       <c r="A97" s="53" t="s">
         <v>313</v>
       </c>
@@ -10225,7 +10439,9 @@
       </c>
       <c r="F97" s="36"/>
       <c r="G97" s="36"/>
-      <c r="H97" s="36"/>
+      <c r="H97" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I97" s="53" t="s">
         <v>18</v>
       </c>
@@ -10250,7 +10466,7 @@
       <c r="Z97" s="45"/>
       <c r="AA97" s="46"/>
     </row>
-    <row r="98" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="19" t="s">
         <v>196</v>
       </c>
@@ -10264,7 +10480,9 @@
       </c>
       <c r="F98" s="21"/>
       <c r="G98" s="21"/>
-      <c r="H98" s="21"/>
+      <c r="H98" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I98" s="19" t="s">
         <v>171</v>
       </c>
@@ -10349,7 +10567,7 @@
       <c r="CC98" s="11"/>
       <c r="CD98" s="11"/>
     </row>
-    <row r="99" spans="1:82" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A99" s="86" t="s">
         <v>196</v>
       </c>
@@ -10365,7 +10583,9 @@
         <v>23</v>
       </c>
       <c r="G99" s="12"/>
-      <c r="H99" s="12"/>
+      <c r="H99" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I99" s="86" t="s">
         <v>40</v>
       </c>
@@ -10403,7 +10623,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="100" spans="1:82" ht="105" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:82" ht="105" x14ac:dyDescent="0.25">
       <c r="A100" s="86" t="s">
         <v>196</v>
       </c>
@@ -10419,7 +10639,9 @@
         <v>23</v>
       </c>
       <c r="G100" s="12"/>
-      <c r="H100" s="12"/>
+      <c r="H100" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I100" s="86" t="s">
         <v>18</v>
       </c>
@@ -10452,7 +10674,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="101" spans="1:82" s="56" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:82" s="56" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="19" t="s">
         <v>305</v>
       </c>
@@ -10464,7 +10686,9 @@
       <c r="E101" s="21"/>
       <c r="F101" s="128"/>
       <c r="G101" s="128"/>
-      <c r="H101" s="128"/>
+      <c r="H101" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I101" s="128" t="s">
         <v>40</v>
       </c>
@@ -10557,7 +10781,7 @@
       <c r="CC101" s="11"/>
       <c r="CD101" s="11"/>
     </row>
-    <row r="102" spans="1:82" s="56" customFormat="1" ht="315" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:82" s="56" customFormat="1" ht="315" x14ac:dyDescent="0.25">
       <c r="A102" s="19" t="s">
         <v>305</v>
       </c>
@@ -10571,7 +10795,9 @@
       </c>
       <c r="F102" s="128"/>
       <c r="G102" s="128"/>
-      <c r="H102" s="128"/>
+      <c r="H102" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I102" s="19" t="s">
         <v>18</v>
       </c>
@@ -10651,7 +10877,7 @@
       <c r="CC102" s="11"/>
       <c r="CD102" s="11"/>
     </row>
-    <row r="103" spans="1:82" ht="60" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:82" ht="60" x14ac:dyDescent="0.25">
       <c r="A103" s="53" t="s">
         <v>305</v>
       </c>
@@ -10669,7 +10895,9 @@
       <c r="G103" s="133" t="s">
         <v>60</v>
       </c>
-      <c r="H103" s="133"/>
+      <c r="H103" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I103" s="133" t="s">
         <v>379</v>
       </c>
@@ -10711,7 +10939,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="104" spans="1:82" ht="60" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:82" ht="60" x14ac:dyDescent="0.25">
       <c r="A104" s="53" t="s">
         <v>305</v>
       </c>
@@ -10723,7 +10951,9 @@
       <c r="E104" s="36"/>
       <c r="F104" s="133"/>
       <c r="G104" s="133"/>
-      <c r="H104" s="133"/>
+      <c r="H104" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I104" s="133" t="s">
         <v>8</v>
       </c>
@@ -10765,7 +10995,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="105" spans="1:82" ht="150" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:82" ht="150" x14ac:dyDescent="0.25">
       <c r="A105" s="53" t="s">
         <v>305</v>
       </c>
@@ -10783,7 +11013,9 @@
       <c r="G105" s="133" t="s">
         <v>60</v>
       </c>
-      <c r="H105" s="133"/>
+      <c r="H105" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I105" s="53" t="s">
         <v>18</v>
       </c>
@@ -10816,7 +11048,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="106" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:82" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="19" t="s">
         <v>305</v>
       </c>
@@ -10832,7 +11064,9 @@
         <v>23</v>
       </c>
       <c r="G106" s="63"/>
-      <c r="H106" s="63"/>
+      <c r="H106" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I106" s="57" t="s">
         <v>366</v>
       </c>
@@ -10925,7 +11159,7 @@
       <c r="CC106" s="11"/>
       <c r="CD106" s="11"/>
     </row>
-    <row r="107" spans="1:82" s="56" customFormat="1" ht="150" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:82" s="56" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A107" s="19" t="s">
         <v>305</v>
       </c>
@@ -10939,7 +11173,9 @@
       </c>
       <c r="F107" s="57"/>
       <c r="G107" s="63"/>
-      <c r="H107" s="63"/>
+      <c r="H107" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I107" s="57" t="s">
         <v>26</v>
       </c>
@@ -11021,7 +11257,7 @@
       <c r="CC107" s="11"/>
       <c r="CD107" s="11"/>
     </row>
-    <row r="108" spans="1:82" s="142" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:82" s="142" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="137" t="s">
         <v>309</v>
       </c>
@@ -11037,7 +11273,9 @@
         <v>23</v>
       </c>
       <c r="G108" s="139"/>
-      <c r="H108" s="139"/>
+      <c r="H108" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I108" s="139"/>
       <c r="J108" s="47"/>
       <c r="K108" s="140"/>
@@ -11071,7 +11309,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="109" spans="1:82" s="142" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:82" s="142" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="137" t="s">
         <v>309</v>
       </c>
@@ -11085,7 +11323,9 @@
       </c>
       <c r="F109" s="36"/>
       <c r="G109" s="139"/>
-      <c r="H109" s="139"/>
+      <c r="H109" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I109" s="53" t="s">
         <v>18</v>
       </c>
@@ -11110,7 +11350,7 @@
       <c r="Z109" s="45"/>
       <c r="AA109" s="138"/>
     </row>
-    <row r="110" spans="1:82" s="145" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:82" s="145" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A110" s="143" t="s">
         <v>311</v>
       </c>
@@ -11124,7 +11364,9 @@
       </c>
       <c r="F110" s="64"/>
       <c r="G110" s="64"/>
-      <c r="H110" s="64"/>
+      <c r="H110" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I110" s="143" t="s">
         <v>137</v>
       </c>
@@ -11227,7 +11469,7 @@
       <c r="CC110" s="142"/>
       <c r="CD110" s="142"/>
     </row>
-    <row r="111" spans="1:82" s="145" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:82" s="145" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="143" t="s">
         <v>311</v>
       </c>
@@ -11239,7 +11481,9 @@
       <c r="E111" s="59"/>
       <c r="F111" s="64"/>
       <c r="G111" s="64"/>
-      <c r="H111" s="64"/>
+      <c r="H111" s="63" t="s">
+        <v>433</v>
+      </c>
       <c r="I111" s="19" t="s">
         <v>18</v>
       </c>
@@ -11319,7 +11563,7 @@
       <c r="CC111" s="142"/>
       <c r="CD111" s="142"/>
     </row>
-    <row r="112" spans="1:82" s="142" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:82" s="142" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="146"/>
       <c r="B112" s="146"/>
       <c r="F112" s="146"/>
@@ -11342,7 +11586,7 @@
       <c r="Z112" s="155"/>
       <c r="AA112" s="156"/>
     </row>
-    <row r="113" spans="5:25" x14ac:dyDescent="0.2">
+    <row r="113" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E113" s="142"/>
       <c r="F113" s="158"/>
       <c r="I113" s="158"/>
@@ -11362,7 +11606,7 @@
       <c r="X113" s="164"/>
       <c r="Y113" s="154"/>
     </row>
-    <row r="114" spans="5:25" x14ac:dyDescent="0.2">
+    <row r="114" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E114" s="142"/>
       <c r="F114" s="158"/>
       <c r="I114" s="158"/>
@@ -11382,7 +11626,7 @@
       <c r="X114" s="164"/>
       <c r="Y114" s="154"/>
     </row>
-    <row r="115" spans="5:25" x14ac:dyDescent="0.2">
+    <row r="115" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E115" s="142"/>
       <c r="F115" s="158"/>
       <c r="I115" s="158"/>
@@ -11402,19 +11646,19 @@
       <c r="X115" s="164"/>
       <c r="Y115" s="154"/>
     </row>
-    <row r="116" spans="5:25" x14ac:dyDescent="0.2">
+    <row r="116" spans="5:25" x14ac:dyDescent="0.25">
       <c r="Y116" s="154"/>
     </row>
-    <row r="117" spans="5:25" x14ac:dyDescent="0.2">
+    <row r="117" spans="5:25" x14ac:dyDescent="0.25">
       <c r="Y117" s="154"/>
     </row>
-    <row r="118" spans="5:25" x14ac:dyDescent="0.2">
+    <row r="118" spans="5:25" x14ac:dyDescent="0.25">
       <c r="Y118" s="154"/>
     </row>
-    <row r="119" spans="5:25" x14ac:dyDescent="0.2">
+    <row r="119" spans="5:25" x14ac:dyDescent="0.25">
       <c r="Y119" s="154"/>
     </row>
-    <row r="120" spans="5:25" x14ac:dyDescent="0.2">
+    <row r="120" spans="5:25" x14ac:dyDescent="0.25">
       <c r="Y120" s="154"/>
     </row>
   </sheetData>
@@ -11506,17 +11750,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.85546875" customWidth="1"/>
-    <col min="2" max="19" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="46.88671875" customWidth="1"/>
+    <col min="2" max="19" width="10.6640625" customWidth="1"/>
     <col min="20" max="20" width="10" customWidth="1"/>
-    <col min="21" max="21" width="46.85546875" customWidth="1"/>
-    <col min="22" max="47" width="10.7109375" customWidth="1"/>
-    <col min="48" max="48" width="4.7109375" customWidth="1"/>
+    <col min="21" max="21" width="46.88671875" customWidth="1"/>
+    <col min="22" max="47" width="10.6640625" customWidth="1"/>
+    <col min="48" max="48" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:47" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>63</v>
       </c>
@@ -11656,7 +11900,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:47" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:47" s="1" customFormat="1" ht="19.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>107</v>
       </c>
@@ -11796,7 +12040,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:47" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:47" s="1" customFormat="1" ht="19.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>81</v>
       </c>
@@ -11936,8 +12180,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:47" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:47" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:47" s="1" customFormat="1" ht="28.65" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:47" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>108</v>
       </c>
@@ -12023,7 +12267,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:47" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:47" s="1" customFormat="1" ht="19.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>107</v>
       </c>
@@ -12109,7 +12353,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:47" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:47" s="1" customFormat="1" ht="19.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>81</v>
       </c>
@@ -12195,8 +12439,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:47" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:47" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:47" s="1" customFormat="1" ht="28.65" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:47" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>114</v>
       </c>
@@ -12288,7 +12532,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:47" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:47" s="1" customFormat="1" ht="19.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>107</v>
       </c>
@@ -12380,7 +12624,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:47" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:47" s="1" customFormat="1" ht="19.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>81</v>
       </c>

</xml_diff>